<commit_message>
Add ability to export excel for description form
</commit_message>
<xml_diff>
--- a/Estimation.WebApi/Forms/SummaryOfEstimation_DetailForm.xlsx
+++ b/Estimation.WebApi/Forms/SummaryOfEstimation_DetailForm.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Summary!$A$1:$H$11</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Summary!$4:$4</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
@@ -118,19 +117,17 @@
       <family val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="AngsanaUPC"/>
+      <family val="1"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="13"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="AngsanaUPC"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -147,7 +144,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -156,31 +153,48 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
@@ -196,105 +210,283 @@
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
       <top/>
       <bottom style="medium">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -614,221 +806,221 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="40.140625" style="3" customWidth="1"/>
-    <col min="3" max="4" width="16.85546875" style="3" customWidth="1"/>
-    <col min="5" max="7" width="23.28515625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="22.7109375" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="17.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="16.85546875" style="2" customWidth="1"/>
+    <col min="5" max="7" width="23.28515625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="2" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" s="7" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" s="5" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9" t="s">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="12"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="13"/>
     </row>
     <row r="6" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="16">
         <v>1</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="18" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9" t="s">
+      <c r="A7" s="14"/>
+      <c r="B7" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="16">
         <v>1</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="18" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="10" t="s">
+      <c r="A8" s="14"/>
+      <c r="B8" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="16">
         <v>1</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="12"/>
+      <c r="H8" s="18"/>
     </row>
     <row r="9" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="19" t="s">
+      <c r="A9" s="14"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="19"/>
-      <c r="E9" s="13" t="s">
+      <c r="D9" s="31"/>
+      <c r="E9" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="12"/>
+      <c r="H9" s="25"/>
     </row>
     <row r="10" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="12"/>
+      <c r="A10" s="23"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="26"/>
     </row>
     <row r="11" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="21" t="s">
+      <c r="A11" s="27"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="16" t="s">
+      <c r="D11" s="33"/>
+      <c r="E11" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="17"/>
+      <c r="H11" s="30"/>
     </row>
     <row r="12" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="1"/>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>